<commit_message>
Add code to git
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>_id</t>
   </si>
@@ -37,22 +37,16 @@
     <t>__v</t>
   </si>
   <si>
-    <t>"6582cd838c005b030256fea2"</t>
-  </si>
-  <si>
-    <t>6582cd348c005b030256fe8f</t>
-  </si>
-  <si>
-    <t>tea</t>
+    <t>"658d37fcd3cb29a14b7efda2"</t>
+  </si>
+  <si>
+    <t>658d37d9d3cb29a14b7efd99</t>
+  </si>
+  <si>
+    <t>this is descii</t>
   </si>
   <si>
     <t>Food</t>
-  </si>
-  <si>
-    <t>"6582d2d38c005b030256fec6"</t>
-  </si>
-  <si>
-    <t>this is</t>
   </si>
 </sst>
 </file>
@@ -430,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -467,7 +461,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -476,38 +470,12 @@
         <v>11</v>
       </c>
       <c r="F3" s="1">
-        <v>45280.471148599536</v>
+        <v>45288.3718136574</v>
       </c>
       <c r="G3" s="1">
-        <v>45280.471148599536</v>
+        <v>45288.3718136574</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1">
-        <v>45280.486892245375</v>
-      </c>
-      <c r="G4" s="1">
-        <v>45280.486892245375</v>
-      </c>
-      <c r="H4">
         <v>0</v>
       </c>
     </row>

</xml_diff>